<commit_message>
update[content email, script sql]
</commit_message>
<xml_diff>
--- a/hcmue/static/resources/output_template_1a.xlsx
+++ b/hcmue/static/resources/output_template_1a.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="121">
   <si>
     <t>Mẫu 1a</t>
   </si>
@@ -67,256 +67,256 @@
     <t>GHI CHÚ</t>
   </si>
   <si>
-    <t>48.01.905.002</t>
-  </si>
-  <si>
-    <t>Nguyễn Hoàng Anh</t>
-  </si>
-  <si>
-    <t>01/09/2004</t>
+    <t>48.01.905.001</t>
+  </si>
+  <si>
+    <t>Ngô Đặng Gia An</t>
+  </si>
+  <si>
+    <t>26/10/2004</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>48.01.905.004</t>
-  </si>
-  <si>
-    <t>Dương Quốc Bảo</t>
-  </si>
-  <si>
-    <t>24/08/2003</t>
-  </si>
-  <si>
-    <t>48.01.905.010</t>
-  </si>
-  <si>
-    <t>Nguyễn Kha Dĩ</t>
-  </si>
-  <si>
-    <t>04/04/2003</t>
-  </si>
-  <si>
-    <t>48.01.905.014</t>
-  </si>
-  <si>
-    <t>Nguyễn Thị Mỹ Duyên</t>
-  </si>
-  <si>
-    <t>11/01/2004</t>
-  </si>
-  <si>
-    <t>48.01.905.017</t>
-  </si>
-  <si>
-    <t>Lê Chí Hoài</t>
-  </si>
-  <si>
-    <t>12/05/2004</t>
-  </si>
-  <si>
-    <t>48.01.905.019</t>
-  </si>
-  <si>
-    <t>Trương Thanh Chí Huân</t>
-  </si>
-  <si>
-    <t>11/05/2004</t>
-  </si>
-  <si>
-    <t>48.01.905.021</t>
-  </si>
-  <si>
-    <t>Trương Quốc Huy</t>
-  </si>
-  <si>
-    <t>01/06/2004</t>
-  </si>
-  <si>
-    <t>48.01.905.023</t>
-  </si>
-  <si>
-    <t>Bùi Lê Ngọc Huyền</t>
-  </si>
-  <si>
-    <t>30/09/2004</t>
-  </si>
-  <si>
-    <t>48.01.905.025</t>
-  </si>
-  <si>
-    <t>Nguyễn Vũ Kha</t>
-  </si>
-  <si>
-    <t>13/05/2004</t>
-  </si>
-  <si>
-    <t>48.01.905.028</t>
-  </si>
-  <si>
-    <t>Nguyễn Minh Khánh</t>
-  </si>
-  <si>
-    <t>20/07/2004</t>
-  </si>
-  <si>
-    <t>48.01.905.030</t>
-  </si>
-  <si>
-    <t>Nguyễn Hoàng Lãm</t>
-  </si>
-  <si>
-    <t>02/12/2004</t>
-  </si>
-  <si>
-    <t>48.01.905.034</t>
-  </si>
-  <si>
-    <t>Châu Thị Ngọc Linh</t>
-  </si>
-  <si>
-    <t>11/07/2004</t>
-  </si>
-  <si>
-    <t>48.01.905.037</t>
-  </si>
-  <si>
-    <t>Lê Thị Cẩm Lụa</t>
-  </si>
-  <si>
-    <t>02/02/2004</t>
-  </si>
-  <si>
-    <t>48.01.905.038</t>
-  </si>
-  <si>
-    <t>Kim Quang Minh</t>
-  </si>
-  <si>
-    <t>14/08/2003</t>
-  </si>
-  <si>
-    <t>48.01.905.041</t>
-  </si>
-  <si>
-    <t>Huỳnh Kim Ngân</t>
-  </si>
-  <si>
-    <t>31/01/2004</t>
-  </si>
-  <si>
-    <t>48.01.905.045</t>
-  </si>
-  <si>
-    <t>Nguyễn Thảo Nguyên</t>
+    <t>48.01.905.005</t>
+  </si>
+  <si>
+    <t>Trần Gia Bảo</t>
   </si>
   <si>
     <t>04/11/2004</t>
   </si>
   <si>
-    <t>48.01.905.047</t>
-  </si>
-  <si>
-    <t>Phan Hoàng Tâm Nhân</t>
-  </si>
-  <si>
-    <t>29/06/2003</t>
-  </si>
-  <si>
-    <t>48.01.905.049</t>
-  </si>
-  <si>
-    <t>Phạm Hiếu Như</t>
-  </si>
-  <si>
-    <t>22/01/2004</t>
-  </si>
-  <si>
-    <t>48.01.905.052</t>
-  </si>
-  <si>
-    <t>Ngô Thị Hồng Phấn</t>
-  </si>
-  <si>
-    <t>14/04/2004</t>
-  </si>
-  <si>
-    <t>48.01.905.055</t>
-  </si>
-  <si>
-    <t>Bùi Minh Tài</t>
-  </si>
-  <si>
-    <t>14/12/2004</t>
-  </si>
-  <si>
-    <t>48.01.905.057</t>
-  </si>
-  <si>
-    <t>Ngô Anh Thắng</t>
-  </si>
-  <si>
-    <t>20/08/2003</t>
-  </si>
-  <si>
-    <t>48.01.905.060</t>
-  </si>
-  <si>
-    <t>Kiều Lệ Thu</t>
-  </si>
-  <si>
-    <t>22/02/2004</t>
-  </si>
-  <si>
-    <t>48.01.905.065</t>
-  </si>
-  <si>
-    <t>Nguyễn Thị Thanh Thúy</t>
-  </si>
-  <si>
-    <t>12/03/2004</t>
-  </si>
-  <si>
-    <t>48.01.905.067</t>
-  </si>
-  <si>
-    <t>Nguyễn Quang Tiến</t>
-  </si>
-  <si>
-    <t>28/09/2000</t>
-  </si>
-  <si>
-    <t>48.01.905.071</t>
-  </si>
-  <si>
-    <t>Lưu Phan Thanh Trang</t>
-  </si>
-  <si>
-    <t>07/05/2004</t>
-  </si>
-  <si>
-    <t>48.01.905.077</t>
-  </si>
-  <si>
-    <t>Lê Hoàng Vũ</t>
-  </si>
-  <si>
-    <t>06/06/2003</t>
-  </si>
-  <si>
-    <t>48.01.905.078</t>
-  </si>
-  <si>
-    <t>Lâm Thảo Vy</t>
+    <t>48.01.905.006</t>
+  </si>
+  <si>
+    <t>Đoàn Thị Kim Chi</t>
+  </si>
+  <si>
+    <t>22/11/2004</t>
+  </si>
+  <si>
+    <t>48.01.905.008</t>
+  </si>
+  <si>
+    <t>Nguyễn Phát Đạt</t>
+  </si>
+  <si>
+    <t>22/03/2004</t>
+  </si>
+  <si>
+    <t>48.01.905.011</t>
+  </si>
+  <si>
+    <t>Danh Hoàng Đức</t>
+  </si>
+  <si>
+    <t>08/01/1999</t>
+  </si>
+  <si>
+    <t>48.01.905.012</t>
+  </si>
+  <si>
+    <t>Văn Hoàng Dương</t>
+  </si>
+  <si>
+    <t>31/05/2004</t>
+  </si>
+  <si>
+    <t>48.01.905.015</t>
+  </si>
+  <si>
+    <t>Nguyễn Hà Giang</t>
+  </si>
+  <si>
+    <t>08/10/2004</t>
+  </si>
+  <si>
+    <t>48.01.905.016</t>
+  </si>
+  <si>
+    <t>Nguyễn Phúc Hậu</t>
+  </si>
+  <si>
+    <t>22/07/2004</t>
+  </si>
+  <si>
+    <t>48.01.905.018</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Hợp</t>
+  </si>
+  <si>
+    <t>20/03/2003</t>
+  </si>
+  <si>
+    <t>48.01.905.024</t>
+  </si>
+  <si>
+    <t>Võ Phương Huỳnh</t>
+  </si>
+  <si>
+    <t>19/03/2004</t>
+  </si>
+  <si>
+    <t>48.01.905.027</t>
+  </si>
+  <si>
+    <t>Đặng Duy Khánh</t>
+  </si>
+  <si>
+    <t>06/08/2004</t>
+  </si>
+  <si>
+    <t>48.01.905.029</t>
+  </si>
+  <si>
+    <t>Nguyễn Minh Đăng Khoa</t>
+  </si>
+  <si>
+    <t>19/02/2002</t>
+  </si>
+  <si>
+    <t>Nghỉ học tạm thời</t>
+  </si>
+  <si>
+    <t>48.01.905.031</t>
+  </si>
+  <si>
+    <t>Trần Kiều Phương Linh</t>
+  </si>
+  <si>
+    <t>13/09/2004</t>
+  </si>
+  <si>
+    <t>48.01.905.040</t>
+  </si>
+  <si>
+    <t>Nguyễn Thanh Nam</t>
+  </si>
+  <si>
+    <t>03/06/2004</t>
+  </si>
+  <si>
+    <t>48.01.905.043</t>
+  </si>
+  <si>
+    <t>Nguyễn Huỳnh Bảo Ngọc</t>
+  </si>
+  <si>
+    <t>48.01.905.044</t>
+  </si>
+  <si>
+    <t>Phạm Thảo Nguyên</t>
+  </si>
+  <si>
+    <t>11/04/2004</t>
+  </si>
+  <si>
+    <t>48.01.905.046</t>
+  </si>
+  <si>
+    <t>Nguyễn Trọng Nhân</t>
+  </si>
+  <si>
+    <t>08/02/2004</t>
+  </si>
+  <si>
+    <t>48.01.905.048</t>
+  </si>
+  <si>
+    <t>Nguyễn Lê Mỹ Nhu</t>
+  </si>
+  <si>
+    <t>15/12/2004</t>
+  </si>
+  <si>
+    <t>48.01.905.054</t>
+  </si>
+  <si>
+    <t>Chiêm Hùng Quan</t>
+  </si>
+  <si>
+    <t>19/06/2004</t>
+  </si>
+  <si>
+    <t>48.01.905.056</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn Tài</t>
+  </si>
+  <si>
+    <t>18/07/1998</t>
+  </si>
+  <si>
+    <t>48.01.905.059</t>
+  </si>
+  <si>
+    <t>Dương Khánh Thoại</t>
+  </si>
+  <si>
+    <t>30/05/2004</t>
+  </si>
+  <si>
+    <t>48.01.905.061</t>
+  </si>
+  <si>
+    <t>Đặng Huỳnh Ngân Thu</t>
+  </si>
+  <si>
+    <t>18/07/2004</t>
+  </si>
+  <si>
+    <t>48.01.905.066</t>
+  </si>
+  <si>
+    <t>Lê Thị Mỹ Tiên</t>
+  </si>
+  <si>
+    <t>09/02/2004</t>
+  </si>
+  <si>
+    <t>48.01.905.068</t>
+  </si>
+  <si>
+    <t>Nguyễn Trần Diễm Trân</t>
   </si>
   <si>
     <t>12/01/2004</t>
   </si>
   <si>
+    <t>48.01.905.070</t>
+  </si>
+  <si>
+    <t>Lâm Thị Thùy Trang</t>
+  </si>
+  <si>
+    <t>26/09/2004</t>
+  </si>
+  <si>
+    <t>48.01.905.072</t>
+  </si>
+  <si>
+    <t>Võ Thanh Trí</t>
+  </si>
+  <si>
+    <t>26/01/2004</t>
+  </si>
+  <si>
+    <t>48.01.905.079</t>
+  </si>
+  <si>
+    <t>Trần Nguyễn Thảo Vy</t>
+  </si>
+  <si>
+    <t>23/03/2004</t>
+  </si>
+  <si>
     <t>Tổng số sinh viên:</t>
   </si>
   <si>
-    <t>182 SV</t>
+    <t>28 SV</t>
   </si>
   <si>
     <t>Xếp loại</t>
@@ -331,7 +331,7 @@
     <t>Xuất sắc</t>
   </si>
   <si>
-    <t>0.00%</t>
+    <t>7.14%</t>
   </si>
   <si>
     <t>Tốt</t>
@@ -340,7 +340,7 @@
     <t>Khá</t>
   </si>
   <si>
-    <t>1.10%</t>
+    <t>14.29%</t>
   </si>
   <si>
     <t>Trung bình</t>
@@ -352,13 +352,16 @@
     <t>Kém</t>
   </si>
   <si>
+    <t>3.57%</t>
+  </si>
+  <si>
     <t>Không xếp loại</t>
   </si>
   <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>21.43%</t>
+    <t>15</t>
+  </si>
+  <si>
+    <t>53.57%</t>
   </si>
   <si>
     <r>
@@ -854,7 +857,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
       <selection activeCell="I14" sqref="I14"/>
@@ -1013,9 +1016,15 @@
       <c r="E12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="F12" s="4">
+        <v>76</v>
+      </c>
+      <c r="G12" s="4">
+        <v>74</v>
+      </c>
+      <c r="H12" s="4">
+        <v>74</v>
+      </c>
       <c r="I12" s="4" t="s">
         <v>20</v>
       </c>
@@ -1034,10 +1043,14 @@
         <v>23</v>
       </c>
       <c r="F13" s="4">
-        <v>69</v>
-      </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+        <v>43</v>
+      </c>
+      <c r="G13" s="4">
+        <v>36</v>
+      </c>
+      <c r="H13" s="4">
+        <v>36</v>
+      </c>
       <c r="I13" s="4" t="s">
         <v>20</v>
       </c>
@@ -1056,10 +1069,14 @@
         <v>26</v>
       </c>
       <c r="F14" s="4">
-        <v>61</v>
-      </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+        <v>92</v>
+      </c>
+      <c r="G14" s="4">
+        <v>92</v>
+      </c>
+      <c r="H14" s="4">
+        <v>92</v>
+      </c>
       <c r="I14" s="4" t="s">
         <v>20</v>
       </c>
@@ -1077,9 +1094,15 @@
       <c r="E15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="F15" s="4">
+        <v>97</v>
+      </c>
+      <c r="G15" s="4">
+        <v>78</v>
+      </c>
+      <c r="H15" s="4">
+        <v>78</v>
+      </c>
       <c r="I15" s="4" t="s">
         <v>20</v>
       </c>
@@ -1097,9 +1120,15 @@
       <c r="E16" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
+      <c r="F16" s="4">
+        <v>94</v>
+      </c>
+      <c r="G16" s="4">
+        <v>81</v>
+      </c>
+      <c r="H16" s="4">
+        <v>92</v>
+      </c>
       <c r="I16" s="4" t="s">
         <v>20</v>
       </c>
@@ -1137,7 +1166,9 @@
       <c r="E18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="4"/>
+      <c r="F18" s="4">
+        <v>76</v>
+      </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4" t="s">
@@ -1177,9 +1208,15 @@
       <c r="E20" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
+      <c r="F20" s="4">
+        <v>31</v>
+      </c>
+      <c r="G20" s="4">
+        <v>18</v>
+      </c>
+      <c r="H20" s="4">
+        <v>18</v>
+      </c>
       <c r="I20" s="4" t="s">
         <v>20</v>
       </c>
@@ -1197,9 +1234,15 @@
       <c r="E21" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
+      <c r="F21" s="4">
+        <v>68</v>
+      </c>
+      <c r="G21" s="4">
+        <v>96</v>
+      </c>
+      <c r="H21" s="4">
+        <v>96</v>
+      </c>
       <c r="I21" s="4" t="s">
         <v>20</v>
       </c>
@@ -1218,12 +1261,14 @@
         <v>50</v>
       </c>
       <c r="F22" s="4">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G22" s="4">
-        <v>62</v>
-      </c>
-      <c r="H22" s="4"/>
+        <v>63</v>
+      </c>
+      <c r="H22" s="4">
+        <v>63</v>
+      </c>
       <c r="I22" s="4" t="s">
         <v>20</v>
       </c>
@@ -1242,14 +1287,10 @@
         <v>53</v>
       </c>
       <c r="F23" s="4"/>
-      <c r="G23" s="4">
-        <v>69</v>
-      </c>
-      <c r="H23" s="4">
-        <v>69</v>
-      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
       <c r="I23" s="4" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" ht="63" customHeight="1" spans="2:9" x14ac:dyDescent="0.25">
@@ -1257,19 +1298,19 @@
         <v>13</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" ht="63" customHeight="1" spans="2:9" x14ac:dyDescent="0.25">
@@ -1277,17 +1318,23 @@
         <v>14</v>
       </c>
       <c r="C25" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="F25" s="4">
         <v>58</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
+      <c r="G25" s="4">
+        <v>58</v>
+      </c>
+      <c r="H25" s="4">
+        <v>58</v>
+      </c>
       <c r="I25" s="4" t="s">
         <v>20</v>
       </c>
@@ -1297,17 +1344,23 @@
         <v>15</v>
       </c>
       <c r="C26" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
+      <c r="F26" s="4">
+        <v>68</v>
+      </c>
+      <c r="G26" s="4">
+        <v>68</v>
+      </c>
+      <c r="H26" s="4">
+        <v>68</v>
+      </c>
       <c r="I26" s="4" t="s">
         <v>20</v>
       </c>
@@ -1317,17 +1370,23 @@
         <v>16</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="F27" s="4">
+        <v>80</v>
+      </c>
+      <c r="G27" s="4">
+        <v>80</v>
+      </c>
+      <c r="H27" s="4">
+        <v>80</v>
+      </c>
       <c r="I27" s="4" t="s">
         <v>20</v>
       </c>
@@ -1337,13 +1396,13 @@
         <v>17</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
@@ -1357,13 +1416,13 @@
         <v>18</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
@@ -1377,13 +1436,13 @@
         <v>19</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
@@ -1397,17 +1456,15 @@
         <v>20</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F31" s="4">
-        <v>52</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4" t="s">
@@ -1419,17 +1476,23 @@
         <v>21</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
+        <v>77</v>
+      </c>
+      <c r="F32" s="4">
+        <v>87</v>
+      </c>
+      <c r="G32" s="4">
+        <v>87</v>
+      </c>
+      <c r="H32" s="4">
+        <v>87</v>
+      </c>
       <c r="I32" s="4" t="s">
         <v>20</v>
       </c>
@@ -1439,13 +1502,13 @@
         <v>22</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
@@ -1459,13 +1522,13 @@
         <v>23</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
@@ -1479,13 +1542,13 @@
         <v>24</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
@@ -1499,13 +1562,13 @@
         <v>25</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
@@ -1519,13 +1582,13 @@
         <v>26</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
@@ -1539,58 +1602,69 @@
         <v>27</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
+      <c r="H38" s="4">
+        <v>6</v>
+      </c>
       <c r="I38" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="7" t="s">
+    <row r="39" ht="63" customHeight="1" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="4">
+        <v>28</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C42" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D41" s="7"/>
-      <c r="E41" t="s">
+      <c r="D42" s="7"/>
+      <c r="E42" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="42" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D42" s="4" t="s">
+    <row r="43" ht="15.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D43" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E43" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="F43" s="4" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D43" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="E43" s="8">
-        <v>0</v>
-      </c>
-      <c r="F43" s="8" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D44" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E44" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F44" s="8" t="s">
         <v>105</v>
@@ -1598,21 +1672,21 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D45" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E45" s="8">
         <v>2</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D46" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E46" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>108</v>
@@ -1620,10 +1694,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D47" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E47" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F47" s="8" t="s">
         <v>105</v>
@@ -1631,10 +1705,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D48" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E48" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F48" s="8" t="s">
         <v>105</v>
@@ -1642,57 +1716,68 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D49" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E49" s="8">
+        <v>1</v>
+      </c>
+      <c r="F49" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="E49" s="8" t="s">
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D50" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="F49" s="8" t="s">
+      <c r="E50" s="8" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="51" ht="93.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
+      <c r="F50" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
-      <c r="I51" s="9"/>
-      <c r="J51" s="9"/>
-      <c r="K51" s="9"/>
-    </row>
-    <row r="53" ht="15.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G53" s="10" t="s">
+    </row>
+    <row r="52" ht="93.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="H53" s="10"/>
-      <c r="I53" s="10"/>
-      <c r="J53" s="10"/>
-      <c r="K53" s="10"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="9"/>
+      <c r="J52" s="9"/>
+      <c r="K52" s="9"/>
     </row>
     <row r="54" ht="15.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="11" t="s">
+      <c r="G54" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="B54" s="11"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="11" t="s">
+      <c r="H54" s="10"/>
+      <c r="I54" s="10"/>
+      <c r="J54" s="10"/>
+      <c r="K54" s="10"/>
+    </row>
+    <row r="55" ht="15.75" customHeight="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="E54" s="11"/>
-      <c r="F54" s="11"/>
-      <c r="G54" s="11" t="s">
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H54" s="11"/>
-      <c r="I54" s="11"/>
-      <c r="J54" s="11"/>
-      <c r="K54" s="11"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H55" s="11"/>
+      <c r="I55" s="11"/>
+      <c r="J55" s="11"/>
+      <c r="K55" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -1704,12 +1789,12 @@
     <mergeCell ref="A7:K7"/>
     <mergeCell ref="A8:K8"/>
     <mergeCell ref="A9:K9"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="A51:K51"/>
-    <mergeCell ref="G53:K53"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="D54:F54"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="A52:K52"/>
     <mergeCell ref="G54:K54"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="D55:F55"/>
+    <mergeCell ref="G55:K55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>